<commit_message>
implemented sending of mails
</commit_message>
<xml_diff>
--- a/prjplanning/Iteration3.xlsx
+++ b/prjplanning/Iteration3.xlsx
@@ -141,7 +141,7 @@
     <t>Iteration 3</t>
   </si>
   <si>
-    <t>(6.12.2012 - 20.12.2012)</t>
+    <t>(6.12.2012 - 14.01.2012) -&gt; Verlängerte Iteration</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,28 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1069,7 +1090,6 @@
             <a:rPr lang="de-CH" sz="2400"/>
             <a:t>6.12.2012 - 20.12.2012</a:t>
           </a:r>
-          <a:endParaRPr lang="de-CH" sz="2400"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -1686,7 +1706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
bug fix concerning updating the ui thread
</commit_message>
<xml_diff>
--- a/prjplanning/Iteration3.xlsx
+++ b/prjplanning/Iteration3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Iterationsplan" sheetId="4" r:id="rId1"/>
@@ -571,39 +571,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1251,11 +1230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91383296"/>
-        <c:axId val="91384832"/>
+        <c:axId val="94266880"/>
+        <c:axId val="94268416"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="91383296"/>
+        <c:axId val="94266880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,7 +1254,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91384832"/>
+        <c:crossAx val="94268416"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="0"/>
@@ -1286,7 +1265,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="91384832"/>
+        <c:axId val="94268416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1318,7 +1297,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91383296"/>
+        <c:crossAx val="94266880"/>
         <c:crossesAt val="41221"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -2049,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,10 +2324,10 @@
       <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="53"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="46" t="s">
         <v>20</v>
       </c>
@@ -2578,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2656,7 +2635,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="I5" s="54">
+      <c r="I5" s="52">
         <f>C5</f>
         <v>16</v>
       </c>
@@ -2678,26 +2657,26 @@
         <v>0</v>
       </c>
       <c r="E6" s="49">
-        <f t="shared" ref="E6:E44" si="0">C6-D6</f>
+        <f t="shared" ref="E6:E43" si="0">C6-D6</f>
         <v>13</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="I6" s="54">
-        <f>I5-TEAM_CAPACITY/$B$43</f>
+      <c r="I6" s="52">
+        <f t="shared" ref="I6:I43" si="1">I5-TEAM_CAPACITY/$B$43</f>
         <v>15.605263157894736</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f t="shared" ref="A7:B44" si="1">A6+1</f>
+        <f t="shared" ref="A7:B43" si="2">A6+1</f>
         <v>41251</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" ref="B7:B19" si="2">B6+1</f>
+        <f t="shared" ref="B7:B19" si="3">B6+1</f>
         <v>2</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" ref="C7:C44" si="3">E6</f>
+        <f t="shared" ref="C7:C44" si="4">E6</f>
         <v>13</v>
       </c>
       <c r="D7" s="7">
@@ -2708,230 +2687,230 @@
         <v>11</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="I7" s="54">
-        <f>I6-TEAM_CAPACITY/$B$43</f>
+      <c r="I7" s="52">
+        <f t="shared" si="1"/>
         <v>15.210526315789473</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41252</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C8" s="7">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="I8" s="52">
+        <f t="shared" si="1"/>
+        <v>14.815789473684209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <f t="shared" si="2"/>
+        <v>41253</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4</v>
+      </c>
+      <c r="E9" s="49">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="I9" s="52">
+        <f t="shared" si="1"/>
+        <v>14.421052631578945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <f t="shared" si="2"/>
+        <v>41254</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="49">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="I10" s="52">
+        <f t="shared" si="1"/>
+        <v>14.026315789473681</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <f t="shared" si="2"/>
+        <v>41255</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="49">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="I11" s="52">
+        <f t="shared" si="1"/>
+        <v>13.631578947368418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f t="shared" si="2"/>
+        <v>41256</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="I12" s="52">
+        <f t="shared" si="1"/>
+        <v>13.236842105263154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <f t="shared" si="2"/>
+        <v>41257</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="I13" s="52">
+        <f t="shared" si="1"/>
+        <v>12.84210526315789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <f t="shared" si="2"/>
+        <v>41258</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="I14" s="52">
+        <f t="shared" si="1"/>
+        <v>12.447368421052627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f t="shared" si="2"/>
+        <v>41259</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="49">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="I15" s="52">
+        <f t="shared" si="1"/>
+        <v>12.052631578947363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <f t="shared" si="2"/>
+        <v>41260</v>
+      </c>
+      <c r="B16" s="3">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="49">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="I8" s="54">
-        <f>I7-TEAM_CAPACITY/$B$43</f>
-        <v>14.815789473684209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <f t="shared" si="1"/>
-        <v>41253</v>
-      </c>
-      <c r="B9" s="3">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="D9" s="7">
-        <v>4</v>
-      </c>
-      <c r="E9" s="49">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="I9" s="54">
-        <f>I8-TEAM_CAPACITY/$B$43</f>
-        <v>14.421052631578945</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <f t="shared" si="1"/>
-        <v>41254</v>
-      </c>
-      <c r="B10" s="3">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="7">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="D10" s="7">
-        <v>0</v>
-      </c>
-      <c r="E10" s="49">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="I10" s="54">
-        <f>I9-TEAM_CAPACITY/$B$43</f>
-        <v>14.026315789473681</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <f t="shared" si="1"/>
-        <v>41255</v>
-      </c>
-      <c r="B11" s="3">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="7">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-      <c r="E11" s="49">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="I11" s="54">
-        <f>I10-TEAM_CAPACITY/$B$43</f>
-        <v>13.631578947368418</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <f t="shared" si="1"/>
-        <v>41256</v>
-      </c>
-      <c r="B12" s="3">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3</v>
-      </c>
-      <c r="E12" s="49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="I12" s="54">
-        <f>I11-TEAM_CAPACITY/$B$43</f>
-        <v>13.236842105263154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <f t="shared" si="1"/>
-        <v>41257</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="I13" s="54">
-        <f>I12-TEAM_CAPACITY/$B$43</f>
-        <v>12.84210526315789</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <f t="shared" si="1"/>
-        <v>41258</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0</v>
-      </c>
-      <c r="E14" s="49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="I14" s="54">
-        <f>I13-TEAM_CAPACITY/$B$43</f>
-        <v>12.447368421052627</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <f t="shared" si="1"/>
-        <v>41259</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="49">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="I15" s="54">
-        <f>I14-TEAM_CAPACITY/$B$43</f>
-        <v>12.052631578947363</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <f t="shared" si="1"/>
-        <v>41260</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
       <c r="C16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D16" s="7">
@@ -2942,22 +2921,22 @@
         <v>4</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="I16" s="54">
-        <f>I15-TEAM_CAPACITY/$B$43</f>
+      <c r="I16" s="52">
+        <f t="shared" si="1"/>
         <v>11.657894736842099</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41261</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D17" s="7">
@@ -2968,22 +2947,22 @@
         <v>4</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="I17" s="54">
-        <f>I16-TEAM_CAPACITY/$B$43</f>
+      <c r="I17" s="52">
+        <f t="shared" si="1"/>
         <v>11.263157894736835</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41262</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D18" s="7">
@@ -2994,22 +2973,22 @@
         <v>4</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="I18" s="54">
-        <f>I17-TEAM_CAPACITY/$B$43</f>
+      <c r="I18" s="52">
+        <f t="shared" si="1"/>
         <v>10.868421052631572</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41263</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D19" s="7">
@@ -3020,14 +2999,14 @@
         <v>4</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="I19" s="54">
-        <f>I18-TEAM_CAPACITY/$B$43</f>
+      <c r="I19" s="52">
+        <f t="shared" si="1"/>
         <v>10.473684210526308</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41264</v>
       </c>
       <c r="B20" s="8">
@@ -3035,7 +3014,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D20" s="7">
@@ -3046,22 +3025,22 @@
         <v>4</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="I20" s="54">
-        <f>I19-TEAM_CAPACITY/$B$43</f>
+      <c r="I20" s="52">
+        <f t="shared" si="1"/>
         <v>10.078947368421044</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41265</v>
       </c>
       <c r="B21" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D21" s="7">
@@ -3071,22 +3050,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I21" s="54">
-        <f>I20-TEAM_CAPACITY/$B$43</f>
+      <c r="I21" s="52">
+        <f t="shared" si="1"/>
         <v>9.6842105263157805</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41266</v>
       </c>
       <c r="B22" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D22" s="7">
@@ -3097,22 +3076,22 @@
         <v>4</v>
       </c>
       <c r="F22" s="12"/>
-      <c r="I22" s="54">
-        <f>I21-TEAM_CAPACITY/$B$43</f>
+      <c r="I22" s="52">
+        <f t="shared" si="1"/>
         <v>9.2894736842105168</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41267</v>
       </c>
       <c r="B23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D23" s="7">
@@ -3123,22 +3102,22 @@
         <v>4</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="I23" s="54">
-        <f>I22-TEAM_CAPACITY/$B$43</f>
+      <c r="I23" s="52">
+        <f t="shared" si="1"/>
         <v>8.8947368421052531</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41268</v>
       </c>
       <c r="B24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D24" s="7">
@@ -3149,22 +3128,22 @@
         <v>4</v>
       </c>
       <c r="F24" s="12"/>
-      <c r="I24" s="54">
-        <f>I23-TEAM_CAPACITY/$B$43</f>
+      <c r="I24" s="52">
+        <f t="shared" si="1"/>
         <v>8.4999999999999893</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41269</v>
       </c>
       <c r="B25" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D25" s="7">
@@ -3175,22 +3154,22 @@
         <v>4</v>
       </c>
       <c r="F25" s="12"/>
-      <c r="I25" s="54">
-        <f>I24-TEAM_CAPACITY/$B$43</f>
+      <c r="I25" s="52">
+        <f t="shared" si="1"/>
         <v>8.1052631578947256</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41270</v>
       </c>
       <c r="B26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D26" s="7">
@@ -3201,22 +3180,22 @@
         <v>4</v>
       </c>
       <c r="F26" s="12"/>
-      <c r="I26" s="54">
-        <f>I25-TEAM_CAPACITY/$B$43</f>
+      <c r="I26" s="52">
+        <f t="shared" si="1"/>
         <v>7.7105263157894628</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41271</v>
       </c>
       <c r="B27" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D27" s="7">
@@ -3227,22 +3206,22 @@
         <v>4</v>
       </c>
       <c r="F27" s="12"/>
-      <c r="I27" s="54">
-        <f>I26-TEAM_CAPACITY/$B$43</f>
+      <c r="I27" s="52">
+        <f t="shared" si="1"/>
         <v>7.3157894736842</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41272</v>
       </c>
       <c r="B28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D28" s="7">
@@ -3253,22 +3232,22 @@
         <v>4</v>
       </c>
       <c r="F28" s="12"/>
-      <c r="I28" s="54">
-        <f>I27-TEAM_CAPACITY/$B$43</f>
+      <c r="I28" s="52">
+        <f t="shared" si="1"/>
         <v>6.9210526315789371</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41273</v>
       </c>
       <c r="B29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D29" s="7">
@@ -3279,22 +3258,22 @@
         <v>4</v>
       </c>
       <c r="F29" s="12"/>
-      <c r="I29" s="54">
-        <f>I28-TEAM_CAPACITY/$B$43</f>
+      <c r="I29" s="52">
+        <f t="shared" si="1"/>
         <v>6.5263157894736743</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41274</v>
       </c>
       <c r="B30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D30" s="7">
@@ -3305,22 +3284,22 @@
         <v>4</v>
       </c>
       <c r="F30" s="12"/>
-      <c r="I30" s="54">
-        <f>I29-TEAM_CAPACITY/$B$43</f>
+      <c r="I30" s="52">
+        <f t="shared" si="1"/>
         <v>6.1315789473684115</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41275</v>
       </c>
       <c r="B31" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D31" s="7">
@@ -3331,22 +3310,22 @@
         <v>4</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="I31" s="54">
-        <f>I30-TEAM_CAPACITY/$B$43</f>
+      <c r="I31" s="52">
+        <f t="shared" si="1"/>
         <v>5.7368421052631486</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41276</v>
       </c>
       <c r="B32" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D32" s="7">
@@ -3356,22 +3335,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I32" s="54">
-        <f>I31-TEAM_CAPACITY/$B$43</f>
+      <c r="I32" s="52">
+        <f t="shared" si="1"/>
         <v>5.3421052631578858</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41277</v>
       </c>
       <c r="B33" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D33" s="7">
@@ -3381,22 +3360,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I33" s="54">
-        <f>I32-TEAM_CAPACITY/$B$43</f>
+      <c r="I33" s="52">
+        <f t="shared" si="1"/>
         <v>4.947368421052623</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41278</v>
       </c>
       <c r="B34" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D34" s="7">
@@ -3406,22 +3385,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I34" s="54">
-        <f>I33-TEAM_CAPACITY/$B$43</f>
+      <c r="I34" s="52">
+        <f t="shared" si="1"/>
         <v>4.5526315789473601</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41279</v>
       </c>
       <c r="B35" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C35" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D35" s="7">
@@ -3431,22 +3410,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I35" s="54">
-        <f>I34-TEAM_CAPACITY/$B$43</f>
+      <c r="I35" s="52">
+        <f t="shared" si="1"/>
         <v>4.1578947368420973</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41280</v>
       </c>
       <c r="B36" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D36" s="7">
@@ -3456,22 +3435,22 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I36" s="54">
-        <f>I35-TEAM_CAPACITY/$B$43</f>
+      <c r="I36" s="52">
+        <f t="shared" si="1"/>
         <v>3.763157894736834</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41281</v>
       </c>
       <c r="B37" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D37" s="7">
@@ -3481,22 +3460,22 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I37" s="54">
-        <f>I36-TEAM_CAPACITY/$B$43</f>
+      <c r="I37" s="52">
+        <f t="shared" si="1"/>
         <v>3.3684210526315708</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41282</v>
       </c>
       <c r="B38" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="C38" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D38" s="7">
@@ -3506,22 +3485,22 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I38" s="54">
-        <f>I37-TEAM_CAPACITY/$B$43</f>
+      <c r="I38" s="52">
+        <f t="shared" si="1"/>
         <v>2.9736842105263075</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41283</v>
       </c>
       <c r="B39" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="C39" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D39" s="7">
@@ -3531,22 +3510,22 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I39" s="54">
-        <f>I38-TEAM_CAPACITY/$B$43</f>
+      <c r="I39" s="52">
+        <f t="shared" si="1"/>
         <v>2.5789473684210442</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41284</v>
       </c>
       <c r="B40" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D40" s="7">
@@ -3556,22 +3535,22 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I40" s="54">
-        <f>I39-TEAM_CAPACITY/$B$43</f>
+      <c r="I40" s="52">
+        <f t="shared" si="1"/>
         <v>2.1842105263157809</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41285</v>
       </c>
       <c r="B41" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D41" s="7">
@@ -3581,22 +3560,22 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I41" s="54">
-        <f>I40-TEAM_CAPACITY/$B$43</f>
+      <c r="I41" s="52">
+        <f t="shared" si="1"/>
         <v>1.7894736842105177</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41286</v>
       </c>
       <c r="B42" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="D42" s="7">
@@ -3606,21 +3585,21 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="54">
-        <f>I41-TEAM_CAPACITY/$B$43</f>
+      <c r="I42" s="52">
+        <f t="shared" si="1"/>
         <v>1.3947368421052544</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41287</v>
       </c>
       <c r="B43" s="8">
         <v>38</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D43" s="7">
@@ -3630,8 +3609,8 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="I43" s="54">
-        <f>I42-TEAM_CAPACITY/$B$43</f>
+      <c r="I43" s="52">
+        <f t="shared" si="1"/>
         <v>0.99999999999999123</v>
       </c>
     </row>
@@ -3644,7 +3623,7 @@
         <v>39</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="D44" s="7">

</xml_diff>